<commit_message>
Better ad placement for exercise pages - Updated media queries and style pages
</commit_message>
<xml_diff>
--- a/Page list.xlsx
+++ b/Page list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5563bf2f66a9f93b/Portfolio-master/Apps/KudosBank revamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7991A69D-1607-4D33-928E-A9010964958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{7991A69D-1607-4D33-928E-A9010964958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A7C2030-6B21-4C57-AFBC-BB5C2BA43295}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1365" windowWidth="29040" windowHeight="15720" xr2:uid="{F31C5384-8139-4C14-BFDD-060202E26079}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F31C5384-8139-4C14-BFDD-060202E26079}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
   <si>
     <t>Category</t>
   </si>
@@ -50,9 +50,6 @@
     <t>ged</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
     <t>GED</t>
   </si>
   <si>
@@ -60,15 +57,6 @@
   </si>
   <si>
     <t>reading-for-meaning</t>
-  </si>
-  <si>
-    <t>Update titles</t>
-  </si>
-  <si>
-    <t>Add meta tags</t>
-  </si>
-  <si>
-    <t>Add Logo</t>
   </si>
   <si>
     <t>Identifying Arguments</t>
@@ -787,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE5B5A7-2673-4DD9-97CF-59BA7483FF28}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
-      <selection activeCell="A108" sqref="A108"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -797,7 +785,7 @@
     <col min="2" max="2" width="17.6328125" customWidth="1"/>
     <col min="3" max="3" width="25.08984375" customWidth="1"/>
     <col min="4" max="4" width="33.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.08984375" customWidth="1"/>
+    <col min="5" max="7" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
@@ -805,13 +793,10 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
@@ -827,8 +812,8 @@
       <c r="E2" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>8</v>
+      <c r="F2" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -836,7 +821,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -844,8 +829,8 @@
       <c r="E3" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
+      <c r="F3" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -853,16 +838,16 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
       <c r="E4" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="F4" t="s">
-        <v>10</v>
+      <c r="F4" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -870,10 +855,13 @@
         <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F5" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -881,10 +869,13 @@
         <v>5</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E6" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F6" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -892,10 +883,13 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E7" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F7" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -903,10 +897,13 @@
         <v>7</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F8" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -914,10 +911,13 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E9" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F9" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -925,10 +925,13 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E10" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F10" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -936,10 +939,13 @@
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E11" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F11" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -947,10 +953,13 @@
         <v>11</v>
       </c>
       <c r="D12" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E12" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F12" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -958,10 +967,13 @@
         <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E13" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F13" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -969,10 +981,13 @@
         <v>13</v>
       </c>
       <c r="D14" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E14" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F14" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -980,10 +995,13 @@
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E15" s="1" t="b">
         <v>1</v>
+      </c>
+      <c r="F15" s="1" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -991,1043 +1009,1322 @@
         <v>15</v>
       </c>
       <c r="D16" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E16" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>16</v>
       </c>
       <c r="D17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E17" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E18" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>18</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E19" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="E20" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>20</v>
       </c>
       <c r="D21" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E21" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>21</v>
       </c>
       <c r="D22" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E22" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>22</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="E23" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>23</v>
       </c>
       <c r="D24" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="E24" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>25</v>
       </c>
       <c r="D26" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E26" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>26</v>
       </c>
       <c r="D27" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E27" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>27</v>
       </c>
       <c r="D28" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E28" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>28</v>
       </c>
       <c r="D29" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E29" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E30" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>30</v>
       </c>
       <c r="D31" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E31" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>31</v>
       </c>
       <c r="D32" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E32" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>32</v>
       </c>
       <c r="D33" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E33" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>33</v>
       </c>
       <c r="D34" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E34" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>34</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E35" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F35" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>35</v>
       </c>
       <c r="C36" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E36" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>36</v>
       </c>
       <c r="D37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E37" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>37</v>
       </c>
       <c r="D38" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E38" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F38" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>38</v>
       </c>
       <c r="D39" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E39" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>39</v>
       </c>
       <c r="D40" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E40" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>40</v>
       </c>
       <c r="D41" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E41" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>41</v>
       </c>
       <c r="D42" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E42" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>42</v>
       </c>
       <c r="D43" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E43" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>43</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E44" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>44</v>
       </c>
       <c r="D45" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E45" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>45</v>
       </c>
       <c r="D46" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E46" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F46" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>46</v>
       </c>
       <c r="D47" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="E47" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>47</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E48" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E49" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E50" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F50" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E51" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F51" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="E52" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E53" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>53</v>
       </c>
       <c r="D54" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E54" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C55" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="E55" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F55" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>55</v>
       </c>
       <c r="D56" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="E56" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F56" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>56</v>
       </c>
       <c r="D57" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E57" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>57</v>
       </c>
       <c r="D58" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E58" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="E59" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>59</v>
       </c>
       <c r="D60" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="E60" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>60</v>
       </c>
       <c r="C61" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E61" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F61" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>61</v>
       </c>
       <c r="D62" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E62" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>62</v>
       </c>
       <c r="D63" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="E63" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F63" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>63</v>
       </c>
       <c r="D64" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E64" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F64" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>64</v>
       </c>
       <c r="C65" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E65" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>65</v>
       </c>
       <c r="D66" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E66" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>66</v>
       </c>
       <c r="D67" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E67" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>67</v>
       </c>
       <c r="D68" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E68" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>68</v>
       </c>
       <c r="C69" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E69" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>69</v>
       </c>
       <c r="D70" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E70" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>70</v>
       </c>
       <c r="D71" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E71" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>71</v>
       </c>
       <c r="D72" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E72" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C73" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E73" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>73</v>
       </c>
       <c r="D74" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E74" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E75" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>75</v>
       </c>
       <c r="D76" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E76" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F76" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>76</v>
       </c>
       <c r="C77" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E77" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F77" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>77</v>
       </c>
       <c r="D78" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E78" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>78</v>
       </c>
       <c r="D79" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E79" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>79</v>
       </c>
       <c r="D80" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E80" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>80</v>
       </c>
       <c r="D81" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E81" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>81</v>
       </c>
       <c r="D82" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E82" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F82" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>82</v>
       </c>
       <c r="D83" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E83" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F83" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>83</v>
       </c>
       <c r="C84" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E84" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>84</v>
       </c>
       <c r="D85" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E85" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F85" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>85</v>
       </c>
       <c r="D86" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E86" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F86" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>86</v>
       </c>
       <c r="D87" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E87" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F87" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>87</v>
       </c>
       <c r="D88" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E88" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>88</v>
       </c>
       <c r="D89" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E89" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>89</v>
       </c>
       <c r="D90" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E90" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F90" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>90</v>
       </c>
       <c r="D91" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E91" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F91" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C92" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E92" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F92" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>92</v>
       </c>
       <c r="D93" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E93" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F93" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>93</v>
       </c>
       <c r="D94" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E94" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F94" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>94</v>
       </c>
       <c r="D95" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E95" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F95" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>95</v>
       </c>
       <c r="D96" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E96" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F96" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>96</v>
       </c>
       <c r="D97" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E97" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F97" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>97</v>
       </c>
       <c r="C98" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E98" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F98" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>98</v>
       </c>
       <c r="D99" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E99" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F99" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>99</v>
       </c>
       <c r="D100" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E100" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F100" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>100</v>
       </c>
       <c r="D101" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E101" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F101" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>101</v>
       </c>
       <c r="D102" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E102" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F102" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>102</v>
       </c>
       <c r="D103" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E103" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F103" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>103</v>
       </c>
       <c r="C104" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E104" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F104" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>104</v>
       </c>
       <c r="D105" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E105" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F105" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>105</v>
       </c>
       <c r="D106" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E106" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F106" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>106</v>
       </c>
       <c r="D107" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E107" s="1" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F107" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E108" s="1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="F108" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E109" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E110" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E111" s="1" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="E112" s="1" t="b">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Meta Descriptions and UI updated for Adsense Ad
</commit_message>
<xml_diff>
--- a/Page list.xlsx
+++ b/Page list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5563bf2f66a9f93b/Portfolio-master/Apps/KudosBank revamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{7991A69D-1607-4D33-928E-A9010964958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5A7C2030-6B21-4C57-AFBC-BB5C2BA43295}"/>
+  <xr:revisionPtr revIDLastSave="76" documentId="8_{7991A69D-1607-4D33-928E-A9010964958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E83A63B8-AAF9-4BBE-863A-65C23091F54A}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F31C5384-8139-4C14-BFDD-060202E26079}"/>
   </bookViews>
@@ -775,8 +775,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE5B5A7-2673-4DD9-97CF-59BA7483FF28}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -813,7 +813,7 @@
         <v>1</v>
       </c>
       <c r="F2" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -830,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -847,7 +847,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -861,7 +861,7 @@
         <v>1</v>
       </c>
       <c r="F5" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -875,7 +875,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -889,7 +889,7 @@
         <v>1</v>
       </c>
       <c r="F7" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -903,7 +903,7 @@
         <v>1</v>
       </c>
       <c r="F8" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -917,7 +917,7 @@
         <v>1</v>
       </c>
       <c r="F9" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -931,7 +931,7 @@
         <v>1</v>
       </c>
       <c r="F10" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -945,7 +945,7 @@
         <v>1</v>
       </c>
       <c r="F11" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
@@ -959,7 +959,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -973,7 +973,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
@@ -987,7 +987,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1001,7 +1001,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1015,7 +1015,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
@@ -1029,7 +1029,7 @@
         <v>1</v>
       </c>
       <c r="F17" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
@@ -1043,7 +1043,7 @@
         <v>1</v>
       </c>
       <c r="F18" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -1057,7 +1057,7 @@
         <v>1</v>
       </c>
       <c r="F19" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -1071,7 +1071,7 @@
         <v>1</v>
       </c>
       <c r="F20" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
@@ -1085,7 +1085,7 @@
         <v>1</v>
       </c>
       <c r="F21" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
@@ -1099,7 +1099,7 @@
         <v>1</v>
       </c>
       <c r="F22" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
@@ -1113,7 +1113,7 @@
         <v>1</v>
       </c>
       <c r="F23" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="F24" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1141,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="F25" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
@@ -1155,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="F26" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
@@ -1169,7 +1169,7 @@
         <v>1</v>
       </c>
       <c r="F27" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1183,7 +1183,7 @@
         <v>1</v>
       </c>
       <c r="F28" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
@@ -1197,7 +1197,7 @@
         <v>1</v>
       </c>
       <c r="F29" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
@@ -1211,7 +1211,7 @@
         <v>1</v>
       </c>
       <c r="F30" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1225,7 +1225,7 @@
         <v>1</v>
       </c>
       <c r="F31" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
@@ -1239,7 +1239,7 @@
         <v>1</v>
       </c>
       <c r="F32" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">
@@ -1253,7 +1253,7 @@
         <v>1</v>
       </c>
       <c r="F33" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1267,7 +1267,7 @@
         <v>1</v>
       </c>
       <c r="F34" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.35">
@@ -1281,7 +1281,7 @@
         <v>1</v>
       </c>
       <c r="F35" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.35">
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
       <c r="F36" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1309,7 +1309,7 @@
         <v>1</v>
       </c>
       <c r="F37" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.35">
@@ -1323,7 +1323,7 @@
         <v>1</v>
       </c>
       <c r="F38" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.35">
@@ -1337,7 +1337,7 @@
         <v>1</v>
       </c>
       <c r="F39" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.35">
@@ -1351,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="F40" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.35">
@@ -1365,7 +1365,7 @@
         <v>1</v>
       </c>
       <c r="F41" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.35">
@@ -1379,7 +1379,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.35">
@@ -1393,7 +1393,7 @@
         <v>1</v>
       </c>
       <c r="F43" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.35">
@@ -1407,7 +1407,7 @@
         <v>1</v>
       </c>
       <c r="F44" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.35">
@@ -1421,7 +1421,7 @@
         <v>1</v>
       </c>
       <c r="F45" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.35">
@@ -1435,7 +1435,7 @@
         <v>1</v>
       </c>
       <c r="F46" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.35">
@@ -1449,7 +1449,7 @@
         <v>1</v>
       </c>
       <c r="F47" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.35">
@@ -1463,7 +1463,7 @@
         <v>1</v>
       </c>
       <c r="F48" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.35">
@@ -1477,7 +1477,7 @@
         <v>1</v>
       </c>
       <c r="F49" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
@@ -1491,7 +1491,7 @@
         <v>1</v>
       </c>
       <c r="F50" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
@@ -1505,7 +1505,7 @@
         <v>1</v>
       </c>
       <c r="F51" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.35">
@@ -1519,7 +1519,7 @@
         <v>1</v>
       </c>
       <c r="F52" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.35">
@@ -1533,7 +1533,7 @@
         <v>1</v>
       </c>
       <c r="F53" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.35">
@@ -1547,7 +1547,7 @@
         <v>1</v>
       </c>
       <c r="F54" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.35">
@@ -1819,7 +1819,7 @@
         <v>1</v>
       </c>
       <c r="F73" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.35">
@@ -1875,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="F77" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
@@ -1973,7 +1973,7 @@
         <v>1</v>
       </c>
       <c r="F84" s="1" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
GED - Science - Scientific Method Resources Added - Commented Meta Descriptions for Exercise Pages
</commit_message>
<xml_diff>
--- a/Page list.xlsx
+++ b/Page list.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5563bf2f66a9f93b/Portfolio-master/Apps/KudosBank revamp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="76" documentId="8_{7991A69D-1607-4D33-928E-A9010964958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E83A63B8-AAF9-4BBE-863A-65C23091F54A}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="8_{7991A69D-1607-4D33-928E-A9010964958C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{79B5D84B-4DF7-44E1-906D-471943B9BB0E}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{F31C5384-8139-4C14-BFDD-060202E26079}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{F31C5384-8139-4C14-BFDD-060202E26079}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="116">
   <si>
     <t>Category</t>
   </si>
@@ -375,6 +376,15 @@
   </si>
   <si>
     <t>Interpretation Practice 3</t>
+  </si>
+  <si>
+    <t>Watch Hour</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Daily Average</t>
   </si>
 </sst>
 </file>
@@ -410,7 +420,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <extLst>
@@ -422,6 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -775,7 +786,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE5B5A7-2673-4DD9-97CF-59BA7483FF28}">
   <dimension ref="A1:F119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
@@ -2368,4 +2379,155 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83928DEA-0955-41AC-A3E2-8DED6A1C3007}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="13.453125" customWidth="1"/>
+    <col min="2" max="2" width="13.26953125" customWidth="1"/>
+    <col min="3" max="3" width="17.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" s="3">
+        <v>45564</v>
+      </c>
+      <c r="B2">
+        <v>2761</v>
+      </c>
+      <c r="C2">
+        <f>B3-B2</f>
+        <v>-2761</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" s="3">
+        <v>45565</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C14" si="0">B4-B3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" s="3">
+        <v>45566</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" s="3">
+        <v>45567</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6" s="3">
+        <v>45568</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>45569</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>45570</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>45571</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>45572</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>45573</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>45574</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>45575</v>
+      </c>
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>45576</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>